<commit_message>
Parsed static data. Database created. SQL Guide created. Github tutorial updated based on feedback
</commit_message>
<xml_diff>
--- a/Dublin Bikes Agile Project.xlsx
+++ b/Dublin Bikes Agile Project.xlsx
@@ -521,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -633,26 +633,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1001,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="2" x14ac:dyDescent="0.35"/>
@@ -1165,7 +1168,7 @@
     </row>
     <row r="7" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="44" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="37" t="s">
@@ -1196,12 +1199,12 @@
     </row>
     <row r="8" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="42" t="s">
+      <c r="B8" s="44"/>
+      <c r="C8" s="40" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="44"/>
+      <c r="E8" s="42"/>
       <c r="F8" s="5"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
@@ -1213,14 +1216,14 @@
     </row>
     <row r="9" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="43" t="s">
+      <c r="B9" s="44"/>
+      <c r="C9" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="44"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="5"/>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -1232,14 +1235,14 @@
     </row>
     <row r="10" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="43" t="s">
+      <c r="B10" s="44"/>
+      <c r="C10" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="44" t="s">
+      <c r="D10" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="44"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="5"/>
       <c r="G10" s="23">
         <v>42805</v>
@@ -1250,7 +1253,7 @@
       <c r="I10" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="J10" s="44" t="s">
+      <c r="J10" s="42" t="s">
         <v>42</v>
       </c>
       <c r="K10" s="5"/>
@@ -1259,14 +1262,14 @@
     </row>
     <row r="11" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="43" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="5"/>
       <c r="G11" s="23">
         <v>42807</v>
@@ -1277,7 +1280,7 @@
       <c r="I11" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="44" t="s">
+      <c r="J11" s="42" t="s">
         <v>42</v>
       </c>
       <c r="K11" s="5"/>
@@ -1286,11 +1289,11 @@
     </row>
     <row r="12" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="43" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="42" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="5"/>
@@ -1301,21 +1304,21 @@
       <c r="H12" s="23">
         <v>42819</v>
       </c>
-      <c r="I12" s="44" t="s">
+      <c r="I12" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="J12" s="44" t="s">
+      <c r="J12" s="42" t="s">
         <v>42</v>
       </c>
       <c r="K12" s="5"/>
-      <c r="L12" s="45" t="s">
+      <c r="L12" s="43" t="s">
         <v>60</v>
       </c>
       <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
-      <c r="B13" s="39"/>
+      <c r="B13" s="44"/>
       <c r="C13" s="24" t="s">
         <v>24</v>
       </c>
@@ -1342,11 +1345,11 @@
     </row>
     <row r="14" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="41" t="s">
+      <c r="B14" s="44"/>
+      <c r="C14" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="42" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="5"/>
@@ -1357,10 +1360,10 @@
       <c r="H14" s="23">
         <v>42815</v>
       </c>
-      <c r="I14" s="44" t="s">
+      <c r="I14" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="J14" s="44" t="s">
+      <c r="J14" s="42" t="s">
         <v>23</v>
       </c>
       <c r="K14" s="5"/>
@@ -1369,7 +1372,7 @@
     </row>
     <row r="15" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
-      <c r="B15" s="39"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="37" t="s">
         <v>44</v>
       </c>
@@ -1387,7 +1390,7 @@
       <c r="I15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="42" t="s">
         <v>58</v>
       </c>
       <c r="K15" s="5"/>
@@ -1396,7 +1399,7 @@
     </row>
     <row r="16" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
-      <c r="B16" s="39"/>
+      <c r="B16" s="44"/>
       <c r="C16" s="37" t="s">
         <v>45</v>
       </c>
@@ -1423,7 +1426,7 @@
     </row>
     <row r="17" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
-      <c r="B17" s="39"/>
+      <c r="B17" s="44"/>
       <c r="C17" s="37" t="s">
         <v>46</v>
       </c>
@@ -1441,18 +1444,18 @@
       <c r="I17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="44"/>
+      <c r="J17" s="42"/>
       <c r="K17" s="5"/>
       <c r="L17" s="8"/>
       <c r="M17" s="5"/>
     </row>
     <row r="18" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="43" t="s">
+      <c r="B18" s="44"/>
+      <c r="C18" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="D18" s="42" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="5"/>
@@ -1460,7 +1463,7 @@
       <c r="G18" s="23"/>
       <c r="H18" s="23"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="44" t="s">
+      <c r="J18" s="42" t="s">
         <v>58</v>
       </c>
       <c r="K18" s="5"/>
@@ -1469,7 +1472,7 @@
     </row>
     <row r="19" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
-      <c r="B19" s="39"/>
+      <c r="B19" s="44"/>
       <c r="C19" s="24" t="s">
         <v>26</v>
       </c>
@@ -1496,11 +1499,11 @@
     </row>
     <row r="20" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="43" t="s">
+      <c r="B20" s="44"/>
+      <c r="C20" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="42" t="s">
         <v>63</v>
       </c>
       <c r="E20" s="5"/>
@@ -1514,7 +1517,7 @@
       <c r="I20" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="J20" s="44" t="s">
+      <c r="J20" s="42" t="s">
         <v>42</v>
       </c>
       <c r="K20" s="5"/>
@@ -1523,11 +1526,11 @@
     </row>
     <row r="21" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="43" t="s">
+      <c r="B21" s="44"/>
+      <c r="C21" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="44" t="s">
+      <c r="D21" s="42" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="5"/>
@@ -1538,10 +1541,10 @@
       <c r="H21" s="23">
         <v>42809</v>
       </c>
-      <c r="I21" s="44" t="s">
+      <c r="I21" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="J21" s="44" t="s">
+      <c r="J21" s="42" t="s">
         <v>42</v>
       </c>
       <c r="K21" s="5"/>
@@ -1550,11 +1553,11 @@
     </row>
     <row r="22" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
-      <c r="B22" s="39"/>
+      <c r="B22" s="44"/>
       <c r="C22" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="44" t="s">
+      <c r="D22" s="42" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="5"/>
@@ -1565,10 +1568,10 @@
       <c r="H22" s="23">
         <v>42809</v>
       </c>
-      <c r="I22" s="44" t="s">
+      <c r="I22" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="44" t="s">
+      <c r="J22" s="42" t="s">
         <v>42</v>
       </c>
       <c r="K22" s="5"/>
@@ -1577,7 +1580,7 @@
     </row>
     <row r="23" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
-      <c r="B23" s="39"/>
+      <c r="B23" s="44"/>
       <c r="C23" s="37" t="s">
         <v>49</v>
       </c>
@@ -1592,10 +1595,10 @@
       <c r="H23" s="23">
         <v>42818</v>
       </c>
-      <c r="I23" s="44" t="s">
+      <c r="I23" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="J23" s="44" t="s">
+      <c r="J23" s="42" t="s">
         <v>42</v>
       </c>
       <c r="K23" s="5"/>
@@ -1604,8 +1607,8 @@
     </row>
     <row r="24" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="43" t="s">
+      <c r="B24" s="44"/>
+      <c r="C24" s="41" t="s">
         <v>59</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -1619,10 +1622,10 @@
       <c r="H24" s="23">
         <v>42818</v>
       </c>
-      <c r="I24" s="44" t="s">
+      <c r="I24" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="J24" s="44" t="s">
+      <c r="J24" s="42" t="s">
         <v>42</v>
       </c>
       <c r="K24" s="5"/>
@@ -1654,7 +1657,7 @@
     </row>
     <row r="26" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="45" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="24" t="s">
@@ -1683,7 +1686,7 @@
     </row>
     <row r="27" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
-      <c r="B27" s="40"/>
+      <c r="B27" s="45"/>
       <c r="C27" s="22" t="s">
         <v>30</v>
       </c>
@@ -1708,7 +1711,7 @@
     </row>
     <row r="28" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
-      <c r="B28" s="40"/>
+      <c r="B28" s="45"/>
       <c r="C28" s="22" t="s">
         <v>32</v>
       </c>
@@ -1733,7 +1736,7 @@
     </row>
     <row r="29" spans="1:13" outlineLevel="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
-      <c r="B29" s="40"/>
+      <c r="B29" s="45"/>
       <c r="C29" s="24" t="s">
         <v>33</v>
       </c>
@@ -1760,7 +1763,7 @@
     </row>
     <row r="30" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
-      <c r="B30" s="40"/>
+      <c r="B30" s="45"/>
       <c r="C30" s="22" t="s">
         <v>34</v>
       </c>
@@ -1787,7 +1790,7 @@
     </row>
     <row r="31" spans="1:13" outlineLevel="2" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
-      <c r="B31" s="40"/>
+      <c r="B31" s="45"/>
       <c r="C31" s="22" t="s">
         <v>35</v>
       </c>

</xml_diff>